<commit_message>
ya no quiero mas
</commit_message>
<xml_diff>
--- a/Barbie_Financiera_FASE_2/BF-0043/BF-0043 - Defectos.xlsx
+++ b/Barbie_Financiera_FASE_2/BF-0043/BF-0043 - Defectos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://esenedusv-my.sharepoint.com/personal/20235894_esen_edu_sv/Documents/PDS/Proyecto/Proyecto-PDS-BarbieFinanciera/Barbie_Financiera_FASE_2/BF-0043/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="29" documentId="8_{9637865A-DA43-4776-8D61-D3B8A2373F56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8580BEB0-E228-438A-80EC-2F088409769F}"/>
+  <xr:revisionPtr revIDLastSave="59" documentId="8_{9637865A-DA43-4776-8D61-D3B8A2373F56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EF6C6C31-3BFA-40F6-8152-936A1A6FABC7}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{64BF1E7B-A780-4405-9CA5-82E133D3DEBF}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
   <si>
     <t>ID DE DEFECTO</t>
   </si>
@@ -83,17 +83,61 @@
     <t>DE-01-CDP-02-BF-0043</t>
   </si>
   <si>
-    <t>Erro al no mostrar la categoria seleccionada</t>
+    <t>Error al no mostrar la categoria seleccionada</t>
+  </si>
+  <si>
+    <t>DE-02-CDP-02-BF-0043</t>
+  </si>
+  <si>
+    <t>Al momento de seleccionar el nombre de la categoria a la cual se desea crear, no aparece en la seccion, y aunque si se crea la categoria con el monto asignado.</t>
+  </si>
+  <si>
+    <t>Que aparezca el nombre de la la categoria en la seccion.</t>
+  </si>
+  <si>
+    <t>No aparece el nombre, pero su funcionalidad para crear la categoria si funciona.</t>
+  </si>
+  <si>
+    <t>Media</t>
+  </si>
+  <si>
+    <t>Abierto</t>
+  </si>
+  <si>
+    <t>Ricardo Cubias</t>
+  </si>
+  <si>
+    <t>1. Acceder a la página principal. 2.Agregar un monto de ingresos. 3. Agregar las categorías de gastos. 4. Agregar una categoría más.</t>
+  </si>
+  <si>
+    <t>DE-03-CDP-02-BF-0043</t>
+  </si>
+  <si>
+    <t>DE-04-CDP-02-BF-0043</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -131,17 +175,31 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -474,10 +532,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12F68637-DEF7-4516-8C03-05513FEFE998}">
-  <dimension ref="A1:N7"/>
+  <dimension ref="A1:N8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="94" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -485,9 +543,9 @@
     <col min="1" max="1" width="24" customWidth="1"/>
     <col min="2" max="2" width="17.42578125" customWidth="1"/>
     <col min="3" max="3" width="25.28515625" customWidth="1"/>
-    <col min="4" max="4" width="31.42578125" customWidth="1"/>
-    <col min="5" max="5" width="20.85546875" customWidth="1"/>
-    <col min="6" max="6" width="23.28515625" customWidth="1"/>
+    <col min="4" max="4" width="26.7109375" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" customWidth="1"/>
+    <col min="6" max="6" width="18.28515625" customWidth="1"/>
     <col min="10" max="10" width="14.28515625" customWidth="1"/>
     <col min="11" max="11" width="20.42578125" customWidth="1"/>
     <col min="12" max="12" width="20" customWidth="1"/>
@@ -539,71 +597,99 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="117.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
+      <c r="C2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" s="4">
+        <v>45605</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>14</v>
+      </c>
       <c r="N2" s="2"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
+    <row r="3" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
+      <c r="A4" s="2" t="s">
+        <v>24</v>
+      </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
+      <c r="A5" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
     </row>
@@ -614,12 +700,12 @@
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
     </row>
@@ -630,16 +716,27 @@
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
     </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="M2" r:id="rId1" xr:uid="{490074EF-1412-4B11-9FC4-07931F1E024B}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>